<commit_message>
Fix excel import and control chart
</commit_message>
<xml_diff>
--- a/examples/data/example_data_with_faults.xlsx
+++ b/examples/data/example_data_with_faults.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">index</t>
   </si>
   <si>
-    <t xml:space="preserve">value (lcl=-7.4 ucl=7.4)</t>
+    <t xml:space="preserve">value</t>
   </si>
 </sst>
 </file>
@@ -40,7 +40,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -100,12 +99,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -122,972 +117,1628 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A4:B122"/>
+  <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A123" activeCellId="0" sqref="A123"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.71"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>7.63866488009365</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>7.04222978169026</v>
+      </c>
+    </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
+      <c r="A4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>7.65771444962803</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>2.31994527085221</v>
+        <v>7.29505891143926</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>1.95909238458065</v>
+        <v>7.08137354401502</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>-0.753841982968344</v>
+        <v>8.45803415833366</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>-3.24366862451913</v>
+        <v>7.52357355562288</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>-3</v>
+        <v>6.06046759662785</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>-2</v>
+        <v>7.86838842300473</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>0.2</v>
+        <v>7.24716238239251</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>0.7</v>
+        <v>7.45100218649346</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>0.83794387909138</v>
+        <v>7.73210816044834</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>1.2</v>
+        <v>7.43192955264933</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>0.874302753873448</v>
+        <v>7.30587000828722</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>4.21119522962876</v>
+        <v>7.62308295558105</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>-3.64564700963497</v>
+        <v>7.38071292007591</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>3</v>
+        <v>7.70109440824764</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>3.37852232321918</v>
+        <v>7.32356097156456</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>-2.6</v>
+        <v>7.91557627850499</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>3</v>
+        <v>7.95990912105601</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>-4.12210200797754</v>
+        <v>7.28743853242633</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>2.6</v>
+        <v>7.88689719999877</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>-2.7</v>
+        <v>8.17303905896634</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>0.899376835647615</v>
+        <v>7.25910911912365</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>4.85801078568726</v>
+        <v>7.28544857055248</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>0.973394031350498</v>
+        <v>7.85943970880373</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>-2.88333003678403</v>
+        <v>7.98125027096929</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>2.53389756171697</v>
+        <v>7.68068931457429</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>-2.45399065399328</v>
+        <v>7.95660376909039</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>-7.85260295716882</v>
+        <v>7.64739895955291</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>2.44345098578806</v>
+        <v>7.35137181746757</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>1.24246538667722</v>
+        <v>8.05708355466491</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>-2.03668545972892</v>
+        <v>7.99639792662296</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>0.363658423954536</v>
+        <v>7.49003540909673</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>3.16646918371305</v>
+        <v>7.54926969940081</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>-2.61257155538862</v>
+        <v>8.2077375768182</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>-2.41028056501556</v>
+        <v>6.95158394345933</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>3.84225683098863</v>
+        <v>6.89808828235854</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>3.15621895280058</v>
+        <v>7.05047385319748</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>-0.647844932573306</v>
+        <v>8.17639728505603</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>7.3283698055003</v>
+        <v>8.08561070872405</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>-0.840488448671855</v>
+        <v>7.53807289259675</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B44" s="0" t="n">
-        <v>-0.699194019395441</v>
+        <v>7.78859897053595</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>1.86531153530793</v>
+        <v>8.38929013976208</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>0.45033535492647</v>
+        <v>7.64233827314942</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>4.86760212832788</v>
+        <v>7.6208068707702</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>4.11343172577636</v>
+        <v>7.6764154317494</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>0.55</v>
+        <v>7.84269770836926</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>0.634982563764348</v>
+        <v>7.59240483595687</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>2.72490578344468</v>
+        <v>7.68318211858003</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>0.28056509226632</v>
+        <v>7.67525580152897</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B53" s="0" t="n">
-        <v>4.1227886036797</v>
+        <v>7.73620310884798</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>-0.73</v>
+        <v>7.85710564068161</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>0.190066590991682</v>
+        <v>7.84373447716403</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B56" s="0" t="n">
-        <v>-2.2</v>
+        <v>7.84432400446009</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B57" s="0" t="n">
-        <v>2.02737541784593</v>
+        <v>7.91015375795383</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>-1.72266404983959</v>
+        <v>8.59097630366652</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>-0.45500252421771</v>
+        <v>7.4513765194352</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B60" s="0" t="n">
-        <v>-0.107793363370619</v>
+        <v>7.37899288595191</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B61" s="0" t="n">
-        <v>2.2</v>
+        <v>7.67977775925602</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>-1.2</v>
+        <v>8.30052520577032</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B63" s="0" t="n">
-        <v>0.521617380811288</v>
+        <v>8.05532379922353</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B64" s="0" t="n">
-        <v>-0.639034616556195</v>
+        <v>8.05657809555879</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B65" s="0" t="n">
-        <v>2.2</v>
+        <v>7.65082399448335</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B66" s="0" t="n">
-        <v>1.42374042905726</v>
+        <v>7.38806302452777</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B67" s="0" t="n">
-        <v>-2.2</v>
+        <v>7.88351093069014</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B68" s="0" t="n">
-        <v>-1.99426112104081</v>
+        <v>7.18943146442794</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B69" s="0" t="n">
-        <v>-1.78908365841114</v>
+        <v>7.85827718353121</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B70" s="0" t="n">
-        <v>-1.05080210486542</v>
+        <v>7.67222543849987</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B71" s="0" t="n">
-        <v>3.38525745954112</v>
+        <v>8.17724054336338</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B72" s="0" t="n">
-        <v>-2.93167289308456</v>
+        <v>7.47594848389749</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B73" s="0" t="n">
-        <v>-2.97448178066489</v>
+        <v>9.54156372593395</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B74" s="0" t="n">
-        <v>-4.17633047434771</v>
+        <v>7.72582829330746</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B75" s="0" t="n">
-        <v>0.889371997460268</v>
+        <v>7.96930627610049</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B76" s="0" t="n">
-        <v>2.46940371367051</v>
+        <v>7.87137773382242</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B77" s="0" t="n">
-        <v>2.12912234134421</v>
+        <v>7.54790700439817</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B78" s="0" t="n">
-        <v>4.31</v>
+        <v>7.38190813361811</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B79" s="0" t="n">
-        <v>-3.61123264235204</v>
+        <v>7.54374494318536</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B80" s="0" t="n">
-        <v>-1.00312601216299</v>
+        <v>7.94441099376255</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B81" s="0" t="n">
-        <v>3.49484289239492</v>
+        <v>9.74857080449032</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B82" s="0" t="n">
-        <v>2</v>
+        <v>7.38518954722709</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B83" s="0" t="n">
-        <v>0.728391787491085</v>
+        <v>7.89368399326381</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B84" s="0" t="n">
-        <v>-3.77744081374519</v>
+        <v>8.40973621975954</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B85" s="0" t="n">
-        <v>6.19618539557649</v>
+        <v>7.68381132980622</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B86" s="0" t="n">
-        <v>-1.95875463839944</v>
+        <v>7.9766810826371</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B87" s="0" t="n">
-        <v>3.81737051225994</v>
+        <v>7.75697230731938</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B88" s="0" t="n">
-        <v>0.454655146144386</v>
+        <v>7.65689566197331</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B89" s="0" t="n">
-        <v>1.90505502531631</v>
+        <v>8.33717144606816</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="n">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B90" s="0" t="n">
-        <v>-4.0703301362344</v>
+        <v>7.4442082020577</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B91" s="0" t="n">
-        <v>-5.63559796972826</v>
+        <v>7.16529848722113</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B92" s="0" t="n">
-        <v>-2.18554877983421</v>
+        <v>7.15393792709021</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B93" s="0" t="n">
-        <v>-2.99891211619025</v>
+        <v>7.45589029860927</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="n">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B94" s="0" t="n">
-        <v>3.19828581754355</v>
+        <v>7.9064740519037</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="n">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B95" s="0" t="n">
-        <v>2.54322463333261</v>
+        <v>6.54366518042532</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="n">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B96" s="0" t="n">
-        <v>2.49087633269158</v>
+        <v>7.99884989752971</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="n">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B97" s="0" t="n">
-        <v>-0.102802794469108</v>
+        <v>7.50227369701293</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="n">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B98" s="0" t="n">
-        <v>-6.50930473763707</v>
+        <v>8.47773131457636</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="n">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B99" s="0" t="n">
-        <v>0.61521944486342</v>
+        <v>5.56557856116307</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="n">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B100" s="0" t="n">
-        <v>-5.19578498189983</v>
+        <v>7.80602403722262</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="n">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B101" s="0" t="n">
-        <v>-1.75987201714374</v>
+        <v>7.35275922122186</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="n">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B102" s="0" t="n">
-        <v>-4.37054255284439</v>
+        <v>7.40304003978743</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="n">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B103" s="0" t="n">
-        <v>3.63584390694209</v>
+        <v>7.88926074705431</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="n">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B104" s="0" t="n">
-        <v>0.323957026168126</v>
+        <v>7.24330126572117</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="n">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B105" s="0" t="n">
-        <v>-2.88333003678403</v>
+        <v>7.75564311762222</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="n">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B106" s="0" t="n">
-        <v>2.53389756171697</v>
+        <v>7.91252438312736</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="n">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B107" s="0" t="n">
-        <v>-2.45399065399328</v>
+        <v>7.44720530051231</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="n">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B108" s="0" t="n">
-        <v>-7.85260295716882</v>
+        <v>7.65555023912434</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="n">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B109" s="0" t="n">
-        <v>2.44345098578806</v>
+        <v>7.99534479275622</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="n">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B110" s="0" t="n">
-        <v>-1.24246538667722</v>
+        <v>8.3855803671883</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="n">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B111" s="0" t="n">
-        <v>2.03668545972892</v>
+        <v>7.18366611767526</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="n">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B112" s="0" t="n">
-        <v>-0.363658423954536</v>
+        <v>7.49993761716764</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="n">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B113" s="0" t="n">
-        <v>3.16646918371305</v>
+        <v>7.47146232365748</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="n">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B114" s="0" t="n">
-        <v>-2.61257155538862</v>
+        <v>7.90821858828302</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="n">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B115" s="0" t="n">
-        <v>2.41028056501556</v>
+        <v>8.10002447928023</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="n">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B116" s="0" t="n">
-        <v>-2.88333003678403</v>
+        <v>7.62047289504982</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="n">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B117" s="0" t="n">
-        <v>2.53389756171697</v>
+        <v>7.35866980257152</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="n">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B118" s="0" t="n">
-        <v>-2.45399065399328</v>
+        <v>7.75778481071714</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="n">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B119" s="0" t="n">
-        <v>2.44345098578806</v>
+        <v>7.65770429529712</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="n">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B120" s="0" t="n">
-        <v>-1.24246538667722</v>
+        <v>7.66814962433143</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="n">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B121" s="0" t="n">
-        <v>2.03668545972892</v>
+        <v>7.60124018746432</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="n">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B122" s="0" t="n">
-        <v>-0.363658423954536</v>
+        <v>8.38481650460149</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="n">
+        <v>121</v>
+      </c>
+      <c r="B123" s="0" t="n">
+        <v>8.07014476129099</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="B124" s="0" t="n">
+        <v>5.81563093973569</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="B125" s="0" t="n">
+        <v>7.39829009527467</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="B126" s="0" t="n">
+        <v>7.71443916643398</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="n">
+        <v>125</v>
+      </c>
+      <c r="B127" s="0" t="n">
+        <v>7.59549019576652</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="n">
+        <v>126</v>
+      </c>
+      <c r="B128" s="0" t="n">
+        <v>6.29162718472105</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="n">
+        <v>127</v>
+      </c>
+      <c r="B129" s="0" t="n">
+        <v>8.03717882366846</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" s="0" t="n">
+        <v>7.88237046224205</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" s="0" t="n">
+        <v>7.58606169113812</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" s="0" t="n">
+        <v>7.60980312536653</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="n">
+        <v>131</v>
+      </c>
+      <c r="B133" s="0" t="n">
+        <v>8.03478495928456</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="n">
+        <v>132</v>
+      </c>
+      <c r="B134" s="0" t="n">
+        <v>7.64023325332505</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="B135" s="0" t="n">
+        <v>8.18706561842352</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="n">
+        <v>134</v>
+      </c>
+      <c r="B136" s="0" t="n">
+        <v>7.44506578894213</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="n">
+        <v>135</v>
+      </c>
+      <c r="B137" s="0" t="n">
+        <v>7.09401882501432</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="n">
+        <v>136</v>
+      </c>
+      <c r="B138" s="0" t="n">
+        <v>7.81334456313196</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="n">
+        <v>137</v>
+      </c>
+      <c r="B139" s="0" t="n">
+        <v>7.3110502192064</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="n">
+        <v>138</v>
+      </c>
+      <c r="B140" s="0" t="n">
+        <v>7.18100306084716</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="n">
+        <v>139</v>
+      </c>
+      <c r="B141" s="0" t="n">
+        <v>7.533244042492</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="B142" s="0" t="n">
+        <v>7.8346474667402</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="n">
+        <v>141</v>
+      </c>
+      <c r="B143" s="0" t="n">
+        <v>8.21406005615669</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="n">
+        <v>142</v>
+      </c>
+      <c r="B144" s="0" t="n">
+        <v>7.75696611231108</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="n">
+        <v>143</v>
+      </c>
+      <c r="B145" s="0" t="n">
+        <v>10.4763335279578</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="n">
+        <v>144</v>
+      </c>
+      <c r="B146" s="0" t="n">
+        <v>7.83558257918577</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="n">
+        <v>145</v>
+      </c>
+      <c r="B147" s="0" t="n">
+        <v>7.61584739015475</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="n">
+        <v>146</v>
+      </c>
+      <c r="B148" s="0" t="n">
+        <v>7.21991971757963</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="B149" s="0" t="n">
+        <v>7.43221943727543</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="B150" s="0" t="n">
+        <v>7.63471791021596</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="n">
+        <v>149</v>
+      </c>
+      <c r="B151" s="0" t="n">
+        <v>7.14389714010445</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="B152" s="0" t="n">
+        <v>7.46369812134658</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="n">
+        <v>151</v>
+      </c>
+      <c r="B153" s="0" t="n">
+        <v>7.85331600588946</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="n">
+        <v>152</v>
+      </c>
+      <c r="B154" s="0" t="n">
+        <v>7.61765427505479</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="n">
+        <v>153</v>
+      </c>
+      <c r="B155" s="0" t="n">
+        <v>5.83845441661235</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="n">
+        <v>154</v>
+      </c>
+      <c r="B156" s="0" t="n">
+        <v>7.67370996913655</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="n">
+        <v>155</v>
+      </c>
+      <c r="B157" s="0" t="n">
+        <v>7.45722416046726</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="n">
+        <v>156</v>
+      </c>
+      <c r="B158" s="0" t="n">
+        <v>7.8242043039722</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="n">
+        <v>157</v>
+      </c>
+      <c r="B159" s="0" t="n">
+        <v>7.66942369176059</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="n">
+        <v>158</v>
+      </c>
+      <c r="B160" s="0" t="n">
+        <v>7.77014524386642</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="n">
+        <v>159</v>
+      </c>
+      <c r="B161" s="0" t="n">
+        <v>7.96363885578213</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="n">
+        <v>160</v>
+      </c>
+      <c r="B162" s="0" t="n">
+        <v>7.54285852425159</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="n">
+        <v>161</v>
+      </c>
+      <c r="B163" s="0" t="n">
+        <v>7.15626876938825</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="n">
+        <v>162</v>
+      </c>
+      <c r="B164" s="0" t="n">
+        <v>4.83804184811642</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="n">
+        <v>163</v>
+      </c>
+      <c r="B165" s="0" t="n">
+        <v>7.93516155623402</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="n">
+        <v>164</v>
+      </c>
+      <c r="B166" s="0" t="n">
+        <v>7.67313645257627</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="n">
+        <v>165</v>
+      </c>
+      <c r="B167" s="0" t="n">
+        <v>8.42717348687942</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="n">
+        <v>166</v>
+      </c>
+      <c r="B168" s="0" t="n">
+        <v>7.99658514310726</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="n">
+        <v>167</v>
+      </c>
+      <c r="B169" s="0" t="n">
+        <v>7.8877445778744</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="n">
+        <v>168</v>
+      </c>
+      <c r="B170" s="0" t="n">
+        <v>7.86347727548202</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="n">
+        <v>169</v>
+      </c>
+      <c r="B171" s="0" t="n">
+        <v>7.48658905614358</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="B172" s="0" t="n">
+        <v>7.08203090974076</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="n">
+        <v>171</v>
+      </c>
+      <c r="B173" s="0" t="n">
+        <v>7.48692245965515</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="n">
+        <v>172</v>
+      </c>
+      <c r="B174" s="0" t="n">
+        <v>7.49221776213302</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="n">
+        <v>173</v>
+      </c>
+      <c r="B175" s="0" t="n">
+        <v>7.90243023021069</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="n">
+        <v>174</v>
+      </c>
+      <c r="B176" s="0" t="n">
+        <v>7.69425347107003</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="n">
+        <v>175</v>
+      </c>
+      <c r="B177" s="0" t="n">
+        <v>7.20320928055433</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="n">
+        <v>176</v>
+      </c>
+      <c r="B178" s="0" t="n">
+        <v>7.63810920309824</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="n">
+        <v>177</v>
+      </c>
+      <c r="B179" s="0" t="n">
+        <v>7.47693464127883</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="n">
+        <v>178</v>
+      </c>
+      <c r="B180" s="0" t="n">
+        <v>7.15730485171402</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="n">
+        <v>179</v>
+      </c>
+      <c r="B181" s="0" t="n">
+        <v>8.10330685352877</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="B182" s="0" t="n">
+        <v>7.88646549255937</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="n">
+        <v>181</v>
+      </c>
+      <c r="B183" s="0" t="n">
+        <v>7.30245980839888</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="n">
+        <v>182</v>
+      </c>
+      <c r="B184" s="0" t="n">
+        <v>7.72870782661243</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="n">
+        <v>183</v>
+      </c>
+      <c r="B185" s="0" t="n">
+        <v>7.56290311731029</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0" t="n">
+        <v>184</v>
+      </c>
+      <c r="B186" s="0" t="n">
+        <v>7.72462651326594</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0" t="n">
+        <v>185</v>
+      </c>
+      <c r="B187" s="0" t="n">
+        <v>7.17446696102233</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="n">
+        <v>186</v>
+      </c>
+      <c r="B188" s="0" t="n">
+        <v>7.83972554793181</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="0" t="n">
+        <v>187</v>
+      </c>
+      <c r="B189" s="0" t="n">
+        <v>7.82893818121859</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="0" t="n">
+        <v>188</v>
+      </c>
+      <c r="B190" s="0" t="n">
+        <v>7.89678550560465</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="0" t="n">
+        <v>189</v>
+      </c>
+      <c r="B191" s="0" t="n">
+        <v>7.83398973742713</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="0" t="n">
+        <v>190</v>
+      </c>
+      <c r="B192" s="0" t="n">
+        <v>7.54763076966348</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="0" t="n">
+        <v>191</v>
+      </c>
+      <c r="B193" s="0" t="n">
+        <v>7.50872865703159</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="0" t="n">
+        <v>192</v>
+      </c>
+      <c r="B194" s="0" t="n">
+        <v>7.4462842583983</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="n">
+        <v>193</v>
+      </c>
+      <c r="B195" s="0" t="n">
+        <v>7.66996671605614</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0" t="n">
+        <v>194</v>
+      </c>
+      <c r="B196" s="0" t="n">
+        <v>7.56065549706719</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="0" t="n">
+        <v>195</v>
+      </c>
+      <c r="B197" s="0" t="n">
+        <v>7.77265607459443</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="0" t="n">
+        <v>196</v>
+      </c>
+      <c r="B198" s="0" t="n">
+        <v>8.22694875772632</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0" t="n">
+        <v>197</v>
+      </c>
+      <c r="B199" s="0" t="n">
+        <v>7.87455910132119</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="0" t="n">
+        <v>198</v>
+      </c>
+      <c r="B200" s="0" t="n">
+        <v>7.48909870718692</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="n">
+        <v>199</v>
+      </c>
+      <c r="B201" s="0" t="n">
+        <v>7.85579636851054</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More accurate control charts
</commit_message>
<xml_diff>
--- a/examples/data/example_data_with_faults.xlsx
+++ b/examples/data/example_data_with_faults.xlsx
@@ -40,6 +40,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -123,11 +124,11 @@
   </sheetPr>
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A157" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B189" activeCellId="0" sqref="B189"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.71"/>
@@ -1578,7 +1579,7 @@
         <v>179</v>
       </c>
       <c r="B181" s="0" t="n">
-        <v>8.10330685352877</v>
+        <v>7.13</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1586,7 +1587,7 @@
         <v>180</v>
       </c>
       <c r="B182" s="0" t="n">
-        <v>7.88646549255937</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1594,7 +1595,7 @@
         <v>181</v>
       </c>
       <c r="B183" s="0" t="n">
-        <v>7.30245980839888</v>
+        <v>7.09</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1602,7 +1603,7 @@
         <v>182</v>
       </c>
       <c r="B184" s="0" t="n">
-        <v>7.72870782661243</v>
+        <v>7.09</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1610,7 +1611,7 @@
         <v>183</v>
       </c>
       <c r="B185" s="0" t="n">
-        <v>7.56290311731029</v>
+        <v>7.08</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1618,7 +1619,7 @@
         <v>184</v>
       </c>
       <c r="B186" s="0" t="n">
-        <v>7.72462651326594</v>
+        <v>7.05</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1626,7 +1627,7 @@
         <v>185</v>
       </c>
       <c r="B187" s="0" t="n">
-        <v>7.17446696102233</v>
+        <v>7</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1634,7 +1635,7 @@
         <v>186</v>
       </c>
       <c r="B188" s="0" t="n">
-        <v>7.83972554793181</v>
+        <v>6.89</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1744,7 +1745,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
More accurate representations of outliers
</commit_message>
<xml_diff>
--- a/examples/data/example_data_with_faults.xlsx
+++ b/examples/data/example_data_with_faults.xlsx
@@ -125,10 +125,10 @@
   <dimension ref="A1:B201"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A157" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B189" activeCellId="0" sqref="B189"/>
+      <selection pane="topLeft" activeCell="B165" activeCellId="0" sqref="B165"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.71"/>
@@ -1451,7 +1451,7 @@
         <v>163</v>
       </c>
       <c r="B165" s="0" t="n">
-        <v>7.93516155623402</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>